<commit_message>
Added more Germans to the List
</commit_message>
<xml_diff>
--- a/Thoughtleader List_GermanSpeaking.xlsx
+++ b/Thoughtleader List_GermanSpeaking.xlsx
@@ -5,25 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\OneDrive\Dokumente\COINS_SwissThoughtleaders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c6ad9d82f21af58/Dokumente/COINS_SwissThoughtleaders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB98D7CC-38A1-45D8-B8F1-8E434B63C793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{BB98D7CC-38A1-45D8-B8F1-8E434B63C793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C7FA891-9F57-4E49-8CBA-756AEFE8B1CB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6285" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabellenblatt1!$A$1:$G$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabellenblatt1!$A$1:$G$47</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -266,13 +277,85 @@
   </si>
   <si>
     <t>Bereich</t>
+  </si>
+  <si>
+    <t>Sophie Passmann</t>
+  </si>
+  <si>
+    <t>@SophiePassmann</t>
+  </si>
+  <si>
+    <t>Sascha Lobo</t>
+  </si>
+  <si>
+    <t>@saschalobo</t>
+  </si>
+  <si>
+    <t>Richard David Precht</t>
+  </si>
+  <si>
+    <t>Oliver Welke</t>
+  </si>
+  <si>
+    <t>Norbert Gstrein</t>
+  </si>
+  <si>
+    <t>Natascha Strobl</t>
+  </si>
+  <si>
+    <t>@Natascha_Strobl</t>
+  </si>
+  <si>
+    <t>Natascha Hoffner</t>
+  </si>
+  <si>
+    <t>@Natschi_Hoffner</t>
+  </si>
+  <si>
+    <t>Mirjam Fischer</t>
+  </si>
+  <si>
+    <t>@Mirjam_Fischer</t>
+  </si>
+  <si>
+    <t>Joyce Ilg</t>
+  </si>
+  <si>
+    <t>@JoyceIlg</t>
+  </si>
+  <si>
+    <t>Joko Winterscheidt</t>
+  </si>
+  <si>
+    <t>@officiallyjoko</t>
+  </si>
+  <si>
+    <t>Jan Böhmermann</t>
+  </si>
+  <si>
+    <t>@janboehm</t>
+  </si>
+  <si>
+    <t>Günther Jauch</t>
+  </si>
+  <si>
+    <t>Frank Thelen</t>
+  </si>
+  <si>
+    <t>@frank_thelen</t>
+  </si>
+  <si>
+    <t>Rezo</t>
+  </si>
+  <si>
+    <t>@rezomusik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,8 +426,19 @@
       <color rgb="FF202122"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Google Sans"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +457,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -372,11 +472,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -422,6 +537,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -640,13 +776,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="D42" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55:I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -656,7 +792,7 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +834,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -717,7 +853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -734,7 +870,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
@@ -749,7 +885,7 @@
       </c>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75">
       <c r="A5" s="12" t="s">
         <v>12</v>
       </c>
@@ -764,7 +900,7 @@
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -779,7 +915,7 @@
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="12.75">
       <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
@@ -798,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="12.75">
       <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
@@ -815,7 +951,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="12.75">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -830,7 +966,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="12.75">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
@@ -845,7 +981,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="12.75">
       <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
@@ -859,7 +995,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="12.75">
       <c r="A12" s="15" t="s">
         <v>21</v>
       </c>
@@ -875,7 +1011,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="12.75">
       <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
@@ -894,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="12.75">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
@@ -911,7 +1047,7 @@
       </c>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:26" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>28</v>
       </c>
@@ -930,7 +1066,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="12.75">
       <c r="A16" s="12" t="s">
         <v>31</v>
       </c>
@@ -947,7 +1083,7 @@
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="13.5" thickBot="1">
       <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
@@ -964,419 +1100,904 @@
       </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A18" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="37">
+        <v>20500</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+    </row>
+    <row r="19" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A19" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="41">
+        <v>44400</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+    </row>
+    <row r="20" spans="1:26" ht="12.75">
+      <c r="A20" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="13">
-        <v>7980</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="19">
-        <v>1910</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="13">
-        <v>15800</v>
+        <v>7980</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="12.75">
       <c r="A21" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="13">
-        <v>2590</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E21" s="19">
+        <v>1910</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:26" ht="12.75">
       <c r="A22" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="13">
-        <v>3640</v>
+        <v>15800</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:26" ht="13.5" thickBot="1">
       <c r="A23" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="19">
-        <v>77400</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>45</v>
+      <c r="E23" s="13">
+        <v>2590</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="13">
-        <v>1090</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="10" t="s">
+    <row r="24" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A24" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="37">
+        <v>54200</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="38" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="13">
-        <v>17400</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="29" t="s">
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="38"/>
+      <c r="X24" s="38"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="38"/>
+    </row>
+    <row r="25" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A25" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="41">
+        <v>12800</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="38" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17">
-        <v>404</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="29" t="s">
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="38"/>
+    </row>
+    <row r="26" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A26" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="37">
+        <v>5730</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17">
-        <v>381</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+    </row>
+    <row r="27" spans="1:26" ht="12.75">
+      <c r="A27" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="13">
+        <v>3640</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="12.75">
       <c r="A28" s="12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="19">
-        <v>24000</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>55</v>
+        <v>77400</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>56</v>
+    <row r="29" spans="1:26" ht="12.75">
+      <c r="A29" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="19">
-        <v>13100</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>57</v>
+      <c r="E29" s="13">
+        <v>1090</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>58</v>
+    <row r="30" spans="1:26" ht="12.75">
+      <c r="A30" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="13">
-        <v>5110</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="13">
-        <v>2100</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="13">
-        <v>7100</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>17400</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="12.75">
+      <c r="A31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17">
+        <v>404</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:26" ht="12.75">
+      <c r="A32" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17">
+        <v>381</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:26" ht="12.75">
       <c r="A33" s="12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="13">
-        <v>16500</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>65</v>
+      <c r="E33" s="19">
+        <v>24000</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="12.75">
+      <c r="A34" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="19">
-        <v>7460</v>
-      </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>13100</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="12.75">
       <c r="A35" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="19">
-        <v>8510</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>67</v>
+      <c r="E35" s="13">
+        <v>5110</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>68</v>
+    <row r="36" spans="1:26" ht="12.75">
+      <c r="A36" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="24">
-        <v>677</v>
-      </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E36" s="13">
+        <v>2100</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:26" ht="12.75">
       <c r="A37" s="12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="13">
-        <v>308</v>
+        <v>7100</v>
       </c>
       <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>71</v>
-      </c>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="1:26" ht="12.75">
+      <c r="A38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="13">
-        <v>20300</v>
+        <v>16500</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="12.75">
       <c r="A39" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="13">
-        <v>669</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="19">
+        <v>7460</v>
+      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:26" ht="12.75">
       <c r="A40" s="12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="13">
-        <v>651</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>76</v>
+      <c r="E40" s="19">
+        <v>8510</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="12.75">
       <c r="A41" s="12" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="13">
+      <c r="E41" s="24">
+        <v>677</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="1:26" ht="26.25" thickBot="1">
+      <c r="A42" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="13">
+        <v>308</v>
+      </c>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A43" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="40">
+        <v>509</v>
+      </c>
+      <c r="F43" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+      <c r="U43" s="38"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="38"/>
+      <c r="X43" s="38"/>
+      <c r="Y43" s="38"/>
+      <c r="Z43" s="38"/>
+    </row>
+    <row r="44" spans="1:26" ht="12.75">
+      <c r="A44" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="13">
+        <v>20300</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:26" ht="12.75">
+      <c r="A45" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="13">
+        <v>669</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:26" ht="12.75">
+      <c r="A46" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="13">
+        <v>651</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:26" ht="13.5" thickBot="1">
+      <c r="A47" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="13">
         <v>41800</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F47" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G47" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A48" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="38"/>
+      <c r="E48" s="40">
+        <v>430</v>
+      </c>
+      <c r="F48" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+      <c r="V48" s="38"/>
+      <c r="W48" s="38"/>
+      <c r="X48" s="38"/>
+      <c r="Y48" s="38"/>
+      <c r="Z48" s="38"/>
+    </row>
+    <row r="49" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A49" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="39">
+        <v>1880</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="38"/>
+      <c r="W49" s="38"/>
+      <c r="X49" s="38"/>
+      <c r="Y49" s="38"/>
+      <c r="Z49" s="38"/>
+    </row>
+    <row r="50" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A50" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="37">
+        <v>3730</v>
+      </c>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38"/>
+      <c r="R50" s="38"/>
+      <c r="S50" s="38"/>
+      <c r="T50" s="38"/>
+      <c r="U50" s="38"/>
+      <c r="V50" s="38"/>
+      <c r="W50" s="38"/>
+      <c r="X50" s="38"/>
+      <c r="Y50" s="38"/>
+      <c r="Z50" s="38"/>
+    </row>
+    <row r="51" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A51" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" s="37">
+        <v>12400</v>
+      </c>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="38"/>
+      <c r="N51" s="38"/>
+      <c r="O51" s="38"/>
+      <c r="P51" s="38"/>
+      <c r="Q51" s="38"/>
+      <c r="R51" s="38"/>
+      <c r="S51" s="38"/>
+      <c r="T51" s="38"/>
+      <c r="U51" s="38"/>
+      <c r="V51" s="38"/>
+      <c r="W51" s="38"/>
+      <c r="X51" s="38"/>
+      <c r="Y51" s="38"/>
+      <c r="Z51" s="38"/>
+    </row>
+    <row r="52" spans="1:26" s="26" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A52" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" s="37">
+        <v>37300</v>
+      </c>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
+      <c r="S52" s="38"/>
+      <c r="T52" s="38"/>
+      <c r="U52" s="38"/>
+      <c r="V52" s="38"/>
+      <c r="W52" s="38"/>
+      <c r="X52" s="38"/>
+      <c r="Y52" s="38"/>
+      <c r="Z52" s="38"/>
+    </row>
+    <row r="53" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A53" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="37">
+        <v>5480</v>
+      </c>
+      <c r="F53" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G53" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="38"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="38"/>
+      <c r="R53" s="38"/>
+      <c r="S53" s="38"/>
+      <c r="T53" s="38"/>
+      <c r="U53" s="38"/>
+      <c r="V53" s="38"/>
+      <c r="W53" s="38"/>
+      <c r="X53" s="38"/>
+      <c r="Y53" s="38"/>
+      <c r="Z53" s="38"/>
+    </row>
+    <row r="54" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A54" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="37">
+        <v>7830</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G54" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
+      <c r="O54" s="38"/>
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38"/>
+      <c r="R54" s="38"/>
+      <c r="S54" s="38"/>
+      <c r="T54" s="38"/>
+      <c r="U54" s="38"/>
+      <c r="V54" s="38"/>
+      <c r="W54" s="38"/>
+      <c r="X54" s="38"/>
+      <c r="Y54" s="38"/>
+      <c r="Z54" s="38"/>
+    </row>
+    <row r="55" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A55" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="37">
+        <v>169000</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
+      <c r="M55" s="38"/>
+      <c r="N55" s="38"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+      <c r="S55" s="38"/>
+      <c r="T55" s="38"/>
+      <c r="U55" s="38"/>
+      <c r="V55" s="38"/>
+      <c r="W55" s="38"/>
+      <c r="X55" s="38"/>
+      <c r="Y55" s="38"/>
+      <c r="Z55" s="38"/>
+    </row>
+    <row r="70" ht="12.75"/>
   </sheetData>
-  <autoFilter ref="A1:G41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G47" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>